<commit_message>
Problemas SAP dispatching y workload
</commit_message>
<xml_diff>
--- a/data/Resultado.xlsx
+++ b/data/Resultado.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="4" customWidth="1" min="2" max="2"/>
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
@@ -493,12 +493,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PR972597</t>
+          <t>PR980926</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BReagan</t>
+          <t>NDINGER</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -511,19 +511,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_US40 (OneSubsea LLC)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PR972452</t>
+          <t>PR980848</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>JJONES75</t>
+          <t>NDINGER</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -536,19 +536,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_US40 (OneSubsea LLC)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PR972488</t>
+          <t>PR980745</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JJONES75</t>
+          <t>KMartinez13</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -568,12 +568,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PR968891</t>
+          <t>PR980825</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CVidrine2</t>
+          <t>JBROUSSARD12</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -593,12 +593,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PR972502</t>
+          <t>PR980719</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>JKramer5</t>
+          <t>RAHRENS2</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -618,12 +618,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PR972585</t>
+          <t>PR980907</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BReagan</t>
+          <t>BBROWN23</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -643,12 +643,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PR972792</t>
+          <t>PR980927</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>JArdoin3</t>
+          <t>JCELESTINE</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -668,12 +668,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PR972669</t>
+          <t>PR980717</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>KMartinez13</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -693,12 +693,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PR972702</t>
+          <t>PR981046</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>LUSCANGA</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -706,24 +706,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_MX10 (Cameron de Mexico)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PR972712</t>
+          <t>PR981066</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>LUSCANGA</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -731,24 +731,24 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_MX10 (Cameron de Mexico)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PR972699</t>
+          <t>PR979733</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GMORENO20</t>
+          <t>MLopez160</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -756,24 +756,24 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_MX10 (Cameron de Mexico)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PR972803</t>
+          <t>PR980732</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -781,24 +781,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PR972728</t>
+          <t>PR980853</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>VAmaral</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -806,24 +806,24 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PR972199</t>
+          <t>PR980803</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>JArdoin3</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -831,24 +831,24 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PR972677</t>
+          <t>PR980832</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GMORENO20</t>
+          <t>VAmaral</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -856,24 +856,24 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PR972750</t>
+          <t>PR979067</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>VAmaral</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -881,24 +881,24 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PR972734</t>
+          <t>PR980824</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>GMORENO20</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -906,24 +906,24 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PR972636</t>
+          <t>PR980808</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>KMartinez13</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -931,24 +931,24 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PR972615</t>
+          <t>PR980868</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BReagan</t>
+          <t>VAmaral</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -956,24 +956,24 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PR972621</t>
+          <t>PR980789</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>KMartinez13</t>
+          <t>VMELLO4</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -981,24 +981,24 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PR972780</t>
+          <t>PR980791</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1006,24 +1006,24 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PR972795</t>
+          <t>PR980763</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1031,24 +1031,24 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PR972273</t>
+          <t>PR980938</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>JBROUSSARD12</t>
+          <t>ISantos24</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1056,24 +1056,24 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PR972642</t>
+          <t>PR980756</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BReagan</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1081,24 +1081,24 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>PR972768</t>
+          <t>PR980940</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>VAmaral</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1106,24 +1106,24 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PR972652</t>
+          <t>PR980750</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>WSACKMANN</t>
+          <t>BMARQUES</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1131,74 +1131,74 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PR972634</t>
+          <t>PR980954</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GMORENO20</t>
+          <t>VMotta</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PR972643</t>
+          <t>PR955335-V5</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>JArdoin3</t>
+          <t>VMotta</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>CAMERON NAM</t>
+          <t>CAMERON LAM</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PR972424</t>
+          <t>PR980560</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>IBorges3</t>
+          <t>TJESUS</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1211,19 +1211,19 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
+          <t>PNP_BR10 (Cameron Tecnologia de Con)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>PR972487</t>
+          <t>PR980733</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>aandrade20</t>
+          <t>TJESUS</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1236,157 +1236,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>PR972506</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>aandrade20</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>CAMERON LAM</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>PR972561</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>VMotta</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>CAMERON LAM</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>PR972605</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>aandrade20</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>CAMERON LAM</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>PR972715</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>LPrado3</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>CAMERON LAM</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>PR972794</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>ESAMPAIO</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>CAMERON LAM</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>PR972806</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>ESAMPAIO</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>CAMERON LAM</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
+          <t>PNP_BR10 (Cameron Tecnologia de Con)</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1251,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1411,13 +1261,13 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="116" customWidth="1" min="9" max="9"/>
+    <col width="61" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
     <col width="38" customWidth="1" min="11" max="11"/>
     <col width="17" customWidth="1" min="12" max="12"/>
@@ -1500,19 +1350,19 @@
     <row r="2">
       <c r="C2" t="inlineStr">
         <is>
-          <t>PR972597</t>
+          <t>PR980926</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bobby Reagan</t>
+          <t>Nicole Dinger</t>
         </is>
       </c>
       <c r="F2" s="3" t="n">
-        <v>46045.58958333333</v>
+        <v>46048.60625</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>46045.58402777778</v>
+        <v>46048.60208333333</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -1521,17 +1371,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>DOGGET- INVOICE: 140263436 - TOYOTA LIFT OF HOUSTON</t>
+          <t>Lafayette Invoice M-402094-TLM</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>$508.08 USD</t>
+          <t>$631.48 USD</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_US40 (OneSubsea LLC)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -1546,19 +1396,19 @@
     <row r="3">
       <c r="C3" t="inlineStr">
         <is>
-          <t>PR972452</t>
+          <t>PR980848</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Casey Jones</t>
+          <t>Nicole Dinger</t>
         </is>
       </c>
       <c r="F3" s="3" t="n">
-        <v>46045.55902777778</v>
+        <v>46048.5875</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>46045.55347222222</v>
+        <v>46048.58611111111</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1567,22 +1417,22 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Evans Equipment - #INV304636</t>
+          <t>McMaster Carr Quote 266816-TLM-Jamie F</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>$616.44 USD</t>
+          <t>$52.60 USD</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_US40 (OneSubsea LLC)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N3" t="n">
@@ -1592,19 +1442,19 @@
     <row r="4">
       <c r="C4" t="inlineStr">
         <is>
-          <t>PR972488</t>
+          <t>PR980745</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Casey Jones</t>
+          <t>Kimberly Martinez</t>
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>46045.56388888889</v>
+        <v>46048.57916666667</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>46045.55972222222</v>
+        <v>46048.56319444445</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1613,12 +1463,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Evans Equipment - #INV304634</t>
+          <t>MSC #30201974</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>$385.98 USD</t>
+          <t>$1,992.92 USD</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -1638,19 +1488,19 @@
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>PR968891</t>
+          <t>PR980825</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Carl Vidrine</t>
+          <t>Joseph Broussard</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>46045.56805555556</v>
+        <v>46048.58680555555</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>46044.69375</v>
+        <v>46048.58055555556</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1659,12 +1509,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2'-6" Sub Face Fixtures, Rings, Mandrals and Collets</t>
+          <t>POWER TOOL SPECIALTIES/ JOB# 201478 &amp; 201379</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>$45,445.00 USD</t>
+          <t>$2,065.00 USD</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1678,25 +1528,25 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" t="inlineStr">
         <is>
-          <t>PR972502</t>
+          <t>PR980719</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Jackson Kramer</t>
+          <t>Robert Ahrens</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
-        <v>46045.57083333333</v>
+        <v>46048.56111111111</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>46045.56180555555</v>
+        <v>46048.55763888889</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1705,12 +1555,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>P&amp;W TICKET-362239</t>
+          <t>Staples</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>$58.60 USD</t>
+          <t>$96.94 USD</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1730,19 +1580,19 @@
     <row r="7">
       <c r="C7" t="inlineStr">
         <is>
-          <t>PR972585</t>
+          <t>PR980907</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Bobby Reagan</t>
+          <t>Brian Brown</t>
         </is>
       </c>
       <c r="F7" s="3" t="n">
-        <v>46045.58333333334</v>
+        <v>46048.60208333333</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>46045.58125</v>
+        <v>46048.59861111111</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1751,12 +1601,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>INV: 54443405 - LINDE GAS</t>
+          <t>1/2" F.F. Lead Figure 1 pk each 0-8</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$430.34 USD</t>
+          <t>$673.97 USD</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1766,7 +1616,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N7" t="n">
@@ -1776,19 +1626,19 @@
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
-          <t>PR972792</t>
+          <t>PR980927</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Joseph Ardoin</t>
+          <t>Joseph Celestine</t>
         </is>
       </c>
       <c r="F8" s="3" t="n">
-        <v>46045.62847222222</v>
+        <v>46048.60416666666</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>46045.62638888889</v>
+        <v>46048.60277777778</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1797,12 +1647,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Industrial Supply 2601-C30749</t>
+          <t>RL-- CMU / V2010B STRETCH WRAP</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>$350.00 USD</t>
+          <t>$2,358.28 USD</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1812,7 +1662,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N8" t="n">
@@ -1822,19 +1672,19 @@
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>PR972669</t>
+          <t>PR980717</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Kimberly Martinez</t>
         </is>
       </c>
       <c r="F9" s="3" t="n">
-        <v>46045.60972222222</v>
+        <v>46048.56180555555</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>46045.59930555556</v>
+        <v>46048.55763888889</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1843,12 +1693,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>#1019829-PRODUCERS</t>
+          <t>TR ENGINEERING #QTE0490</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>$2,478.76 USD</t>
+          <t>$3,580.00 USD</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1868,19 +1718,19 @@
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t>PR972702</t>
+          <t>PR981046</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Luis Alfonso Hernandez</t>
         </is>
       </c>
       <c r="F10" s="3" t="n">
-        <v>46045.61805555555</v>
+        <v>46048.63194444445</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>46045.60972222222</v>
+        <v>46048.62708333333</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1889,17 +1739,17 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>#1019837-PRODUCERS</t>
+          <t>Plug Gage 1 1/2"-11 1/2 NPT</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>$1,964.52 USD</t>
+          <t>$1.00 USD</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_MX10 (Cameron de Mexico)</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1914,19 +1764,19 @@
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>PR972712</t>
+          <t>PR981066</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Luis Alfonso Hernandez</t>
         </is>
       </c>
       <c r="F11" s="3" t="n">
-        <v>46045.61527777778</v>
+        <v>46048.63472222222</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>46045.61180555556</v>
+        <v>46048.63263888889</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1935,17 +1785,17 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>#1019838-PRODUCERS</t>
+          <t>Plug Gage 1"-11 1/2 NPT</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>$2,454.39 USD</t>
+          <t>$1.00 USD</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_MX10 (Cameron de Mexico)</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1960,19 +1810,19 @@
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>PR972699</t>
+          <t>PR979733</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Guadalupe Moreno</t>
+          <t>Monsserrath Lopez</t>
         </is>
       </c>
       <c r="F12" s="3" t="n">
-        <v>46045.61527777778</v>
+        <v>46048.56041666667</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>46045.60902777778</v>
+        <v>46048.42013888889</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1981,22 +1831,22 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>P&amp;W - 0363705</t>
+          <t>TAQUIZA DIAS SIN ACCIDENTES</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>$1,458.45 USD</t>
+          <t>$4,163.01 USD</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_MX10 (Cameron de Mexico)</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N12" t="n">
@@ -2006,19 +1856,19 @@
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>PR972803</t>
+          <t>PR980732</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F13" s="3" t="n">
-        <v>46045.62916666667</v>
+        <v>46048.56180555555</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>46045.62847222222</v>
+        <v>46048.56041666667</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -2027,22 +1877,22 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>#1882A-NAM</t>
+          <t>RC COTAÇÃO- Kendex OCTG Orange</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>$4,800.00 USD</t>
+          <t>R$2.00 BRL</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N13" t="n">
@@ -2052,19 +1902,19 @@
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t>PR972728</t>
+          <t>PR980853</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Vitor Marcos Silva Amaral</t>
         </is>
       </c>
       <c r="F14" s="3" t="n">
-        <v>46045.61736111111</v>
+        <v>46048.59097222222</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>46045.61527777778</v>
+        <v>46048.5875</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -2073,22 +1923,22 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>#1019841-PRODUCERS</t>
+          <t>Medição de área Triunfo - IRS7 - Setembro/2025</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>$715.24 USD</t>
+          <t>$66,165.94 USD</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N14" t="n">
@@ -2098,19 +1948,19 @@
     <row r="15">
       <c r="C15" t="inlineStr">
         <is>
-          <t>PR972199</t>
+          <t>PR980803</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Joseph Ardoin</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F15" s="3" t="n">
-        <v>46045.62222222222</v>
+        <v>46048.57569444444</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>46045.50347222222</v>
+        <v>46048.575</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -2119,22 +1969,22 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Industrial Supply 2601-c30737</t>
+          <t>RC COTAÇÃO-Graxa Multiuso Molygrafit - GLI-2/B Branca</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>$50.00 USD</t>
+          <t>R$4.00 BRL</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N15" t="n">
@@ -2144,19 +1994,19 @@
     <row r="16">
       <c r="C16" t="inlineStr">
         <is>
-          <t>PR972677</t>
+          <t>PR980832</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Guadalupe Moreno</t>
+          <t>Vitor Marcos Silva Amaral</t>
         </is>
       </c>
       <c r="F16" s="3" t="n">
-        <v>46045.60833333333</v>
+        <v>46048.5875</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>46045.60069444445</v>
+        <v>46048.58263888889</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -2165,22 +2015,22 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>P&amp;W Sales - 0361126</t>
+          <t>Medição de área Triunfo - IRS7 - Outubro/2025</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>$570.15 USD</t>
+          <t>$68,341.09 USD</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N16" t="n">
@@ -2190,19 +2040,19 @@
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t>PR972750</t>
+          <t>PR979067</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Vitor Marcos Silva Amaral</t>
         </is>
       </c>
       <c r="F17" s="3" t="n">
-        <v>46045.62430555555</v>
+        <v>46048.58263888889</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>46045.62013888889</v>
+        <v>46048.35208333333</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -2211,17 +2061,17 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>#1879-NAM</t>
+          <t>Medição de área Triunfo - IRS7 - Novembro/2025</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>$4,800.00 USD</t>
+          <t>$69,821.27 USD</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -2236,19 +2086,19 @@
     <row r="18">
       <c r="C18" t="inlineStr">
         <is>
-          <t>PR972734</t>
+          <t>PR980824</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Guadalupe Moreno</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F18" s="3" t="n">
-        <v>46045.62430555555</v>
+        <v>46048.58125</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>46045.61597222222</v>
+        <v>46048.58055555556</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -2257,17 +2107,17 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Torcup - 119429</t>
+          <t>RC COTAÇÃO-Partícula magnética ML-500WB</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>$1,998.00 USD</t>
+          <t>R$2.00 BRL</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -2282,19 +2132,19 @@
     <row r="19">
       <c r="C19" t="inlineStr">
         <is>
-          <t>PR972636</t>
+          <t>PR980808</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Kimberly Martinez</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F19" s="3" t="n">
-        <v>46045.60277777778</v>
+        <v>46048.57777777778</v>
       </c>
       <c r="G19" s="3" t="n">
-        <v>46045.59305555555</v>
+        <v>46048.57638888889</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -2303,22 +2153,22 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>SAFETY KLEEN #99022640</t>
+          <t>RC COTAÇÃO- Penetrante SKL-WP2</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>$408.13 USD</t>
+          <t>R$24.00 BRL</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N19" t="n">
@@ -2328,19 +2178,19 @@
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>PR972615</t>
+          <t>PR980868</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Bobby Reagan</t>
+          <t>Vitor Marcos Silva Amaral</t>
         </is>
       </c>
       <c r="F20" s="3" t="n">
-        <v>46045.58888888889</v>
+        <v>46048.59375</v>
       </c>
       <c r="G20" s="3" t="n">
-        <v>46045.58680555555</v>
+        <v>46048.59097222222</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -2349,17 +2199,17 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>DOGGET- INVOICE: 140263438 - TOYOTA LIFT OF HOUSTON</t>
+          <t>Medição de área Triunfo - IRS7 - Agosto/2025</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>$791.00 USD</t>
+          <t>$63,539.52 USD</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -2374,19 +2224,19 @@
     <row r="21">
       <c r="C21" t="inlineStr">
         <is>
-          <t>PR972621</t>
+          <t>PR980789</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Kimberly Martinez</t>
+          <t>Victor Miranda Mello</t>
         </is>
       </c>
       <c r="F21" s="3" t="n">
-        <v>46045.59166666667</v>
+        <v>46048.57569444444</v>
       </c>
       <c r="G21" s="3" t="n">
-        <v>46045.58888888889</v>
+        <v>46048.57222222222</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -2395,22 +2245,22 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>CINTAS #4256987118</t>
+          <t>Headset for macaé team</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>$45.00 USD</t>
+          <t>$216.25 USD</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N21" t="n">
@@ -2420,19 +2270,19 @@
     <row r="22">
       <c r="C22" t="inlineStr">
         <is>
-          <t>PR972780</t>
+          <t>PR980791</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F22" s="3" t="n">
-        <v>46045.62708333333</v>
+        <v>46048.57361111111</v>
       </c>
       <c r="G22" s="3" t="n">
-        <v>46045.625</v>
+        <v>46048.57291666666</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -2441,22 +2291,22 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>#1880B-NAM</t>
+          <t>RC COTAÇÃO- Revelador SKD-S2</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>$3,600.00 USD</t>
+          <t>R$48.00 BRL</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N22" t="n">
@@ -2466,19 +2316,19 @@
     <row r="23">
       <c r="C23" t="inlineStr">
         <is>
-          <t>PR972795</t>
+          <t>PR980763</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F23" s="3" t="n">
-        <v>46045.62777777778</v>
+        <v>46048.57083333333</v>
       </c>
       <c r="G23" s="3" t="n">
-        <v>46045.62708333333</v>
+        <v>46048.56736111111</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -2487,22 +2337,22 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>#1881-NAM</t>
+          <t>RC COTAÇÃO-Transdutor K2G Ø24 - ângulo 0 - Frequência 2 MHz</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>$4,800.00 USD</t>
+          <t>R$2.00 BRL</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N23" t="n">
@@ -2512,19 +2362,19 @@
     <row r="24">
       <c r="C24" t="inlineStr">
         <is>
-          <t>PR972273</t>
+          <t>PR980938</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Joseph Broussard</t>
+          <t>Isabel Cristina Dos Santos</t>
         </is>
       </c>
       <c r="F24" s="3" t="n">
-        <v>46045.59236111111</v>
+        <v>46048.64305555556</v>
       </c>
       <c r="G24" s="3" t="n">
-        <v>46045.51875</v>
+        <v>46048.60486111111</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -2533,17 +2383,17 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>NI WELDING SUPPLY /ORD.# 10610244-00</t>
+          <t>Pedido fechamento Transmaz Dezembro</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>$797.00 USD</t>
+          <t>$7,482.32 USD</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2558,19 +2408,19 @@
     <row r="25">
       <c r="C25" t="inlineStr">
         <is>
-          <t>PR972642</t>
+          <t>PR980756</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Bobby Reagan</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F25" s="3" t="n">
-        <v>46045.59722222222</v>
+        <v>46048.56666666667</v>
       </c>
       <c r="G25" s="3" t="n">
-        <v>46045.59375</v>
+        <v>46048.56527777778</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -2579,22 +2429,22 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>DOGGET- INVOICE: 140263435 - TOYOTA LIFT OF HOUSTON</t>
+          <t>RC COTAÇÃO- Korr Guard</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>$1,017.69 USD</t>
+          <t>R$2.00 BRL</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N25" t="n">
@@ -2604,19 +2454,19 @@
     <row r="26">
       <c r="C26" t="inlineStr">
         <is>
-          <t>PR972768</t>
+          <t>PR980940</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Vitor Marcos Silva Amaral</t>
         </is>
       </c>
       <c r="F26" s="3" t="n">
-        <v>46045.62430555555</v>
+        <v>46048.60763888889</v>
       </c>
       <c r="G26" s="3" t="n">
-        <v>46045.62291666667</v>
+        <v>46048.60486111111</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -2625,17 +2475,17 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>#1880A-NAM</t>
+          <t>Medição de área Triunfo - IRS7 - Julho/2025</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>$4,800.00 USD</t>
+          <t>$70,525.26 USD</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2650,19 +2500,19 @@
     <row r="27">
       <c r="C27" t="inlineStr">
         <is>
-          <t>PR972652</t>
+          <t>PR980750</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>William Sackmann</t>
+          <t>Bruno De Souza Marques</t>
         </is>
       </c>
       <c r="F27" s="3" t="n">
-        <v>46045.59861111111</v>
+        <v>46048.56527777778</v>
       </c>
       <c r="G27" s="3" t="n">
-        <v>46045.59513888889</v>
+        <v>46048.56388888889</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -2671,22 +2521,22 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>#1413-ITS BEEN TOO LONG CLEANING</t>
+          <t>RC COTAÇÃO-Cotação de Rust Veto AS EU</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>$800.00 USD</t>
+          <t>R$2.00 BRL</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N27" t="n">
@@ -2696,19 +2546,19 @@
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
-          <t>PR972634</t>
+          <t>PR980954</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Guadalupe Moreno</t>
+          <t>VITOR ARAUJO MOTTA</t>
         </is>
       </c>
       <c r="F28" s="3" t="n">
-        <v>46045.60069444445</v>
+        <v>46048.61041666667</v>
       </c>
       <c r="G28" s="3" t="n">
-        <v>46045.59236111111</v>
+        <v>46048.60833333333</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -2717,17 +2567,17 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>P&amp;W - 0362907</t>
+          <t>URG SLSS/TLM/COTIMA QUOTE 274692</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>$1,753.65 USD</t>
+          <t>$1,440.18 USD</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2742,19 +2592,19 @@
     <row r="29">
       <c r="C29" t="inlineStr">
         <is>
-          <t>PR972643</t>
+          <t>PR955335-V5</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Joseph Ardoin</t>
+          <t>VITOR ARAUJO MOTTA</t>
         </is>
       </c>
       <c r="F29" s="3" t="n">
-        <v>46045.60138888889</v>
+        <v>46048.60972222222</v>
       </c>
       <c r="G29" s="3" t="n">
-        <v>46045.59375</v>
+        <v>46045.52777777778</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -2763,17 +2613,17 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Element ELA575554IN</t>
+          <t>URG SLSS/EQN BACALHAU/DISMETER QUOTE 50409</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>$160.00 USD</t>
+          <t>$374.73 USD</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>PNP_US10 (Cameron Intl Corp)</t>
+          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2782,25 +2632,25 @@
         </is>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="C30" t="inlineStr">
         <is>
-          <t>PR972424</t>
+          <t>PR980560</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Iago Oliveira Melo Borges</t>
+          <t>Tiago Oliveira De Jesus</t>
         </is>
       </c>
       <c r="F30" s="3" t="n">
-        <v>46045.55416666667</v>
+        <v>46048.56041666667</v>
       </c>
       <c r="G30" s="3" t="n">
-        <v>46045.54722222222</v>
+        <v>46048.53055555555</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -2809,17 +2659,17 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Laptop Vanessa</t>
+          <t>PC request Lais</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>$3,975.00 USD</t>
+          <t>R$6,221.62 BRL</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
+          <t>PNP_BR10 (Cameron Tecnologia de Con)</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2834,19 +2684,19 @@
     <row r="31">
       <c r="C31" t="inlineStr">
         <is>
-          <t>PR972487</t>
+          <t>PR980733</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Amanda Silva De Andrade</t>
+          <t>Tiago Oliveira De Jesus</t>
         </is>
       </c>
       <c r="F31" s="3" t="n">
-        <v>46045.5625</v>
+        <v>46048.56319444445</v>
       </c>
       <c r="G31" s="3" t="n">
-        <v>46045.55902777778</v>
+        <v>46048.56111111111</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2855,17 +2705,17 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>OP26-093 RESISTENCIA SMS 380/220V 8.5KW</t>
+          <t>docksataion</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>$1,012.16 USD</t>
+          <t>R$1,522.68 BRL</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
+          <t>PNP_BR10 (Cameron Tecnologia de Con)</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2874,282 +2724,6 @@
         </is>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>PR972506</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Amanda Silva De Andrade</t>
-        </is>
-      </c>
-      <c r="F32" s="3" t="n">
-        <v>46045.57569444444</v>
-      </c>
-      <c r="G32" s="3" t="n">
-        <v>46045.56319444445</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>OP26-110 "N° PROPOSTA: VTP3744-25 MATERIAL PARA CORREÇÃO DE PENDÊNCIA LEVANTADA NA MANUTENÇAÕ PREVENTIVA DA MAP 03</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>$1,281.62 USD</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>PR972561</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>VITOR ARAUJO MOTTA</t>
-        </is>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>46045.58263888889</v>
-      </c>
-      <c r="G33" s="3" t="n">
-        <v>46045.575</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>URG SLSS/TLM/STEELFORM TEC LOG DEZ-25</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>$2,616.02 USD</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>PR972605</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Amanda Silva De Andrade</t>
-        </is>
-      </c>
-      <c r="F34" s="3" t="n">
-        <v>46045.59513888889</v>
-      </c>
-      <c r="G34" s="3" t="n">
-        <v>46045.58541666667</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>OP26-112 BM143 - PREVENTIVA MAP16 E MAP14</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>$1,751.18 USD</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>PR972715</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Liryel Aguiar Prado</t>
-        </is>
-      </c>
-      <c r="F35" s="3" t="n">
-        <v>46045.62222222222</v>
-      </c>
-      <c r="G35" s="3" t="n">
-        <v>46045.6125</v>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>PLUG MACHO P/CONEXAO 3/4" OD INOX FITOK</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>$142.54 USD</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>PR972794</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Evandro Luiz Sampaio</t>
-        </is>
-      </c>
-      <c r="F36" s="3" t="n">
-        <v>46045.62847222222</v>
-      </c>
-      <c r="G36" s="3" t="n">
-        <v>46045.62708333333</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>ETIQUETAS</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>$194.95 USD</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>PR972806</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Evandro Luiz Sampaio</t>
-        </is>
-      </c>
-      <c r="F37" s="3" t="n">
-        <v>46045.62986111111</v>
-      </c>
-      <c r="G37" s="3" t="n">
-        <v>46045.62916666667</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>ETIQUETAS</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>$194.95 USD</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>PNP_BR11 (OneSubsea do Brasil Servi)</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N37" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>